<commit_message>
Confirmation box for add new User
</commit_message>
<xml_diff>
--- a/recruit/src/main/resources/Candidates-wordformat.xlsx
+++ b/recruit/src/main/resources/Candidates-wordformat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="825">
   <si>
     <t xml:space="preserve">New Candidates</t>
   </si>
@@ -1683,15 +1683,6 @@
     <t xml:space="preserve">ITIL, Switches, VPN, Cloud, CISCO, SOC, MOTIV, LDAP, RSA</t>
   </si>
   <si>
-    <t xml:space="preserve">C122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile, UAT, ISTQB, TDD, Test Strategy, Selenium, SoapUI, LoadRunner, Jmeter</t>
-  </si>
-  <si>
     <t xml:space="preserve">C121</t>
   </si>
   <si>
@@ -2446,15 +2437,6 @@
   </si>
   <si>
     <t xml:space="preserve">Java, C#, Spring, Soap, Rest, Agile, mySQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full stack Java / Dev ops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpringBoot, REST, Eclipse, Hibernat, Docker, Kubenetis</t>
   </si>
   <si>
     <t xml:space="preserve">C15</t>
@@ -2821,10 +2803,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:BL1048576"/>
+  <dimension ref="A2:BL276"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8633,28 +8615,28 @@
         <v>21</v>
       </c>
       <c r="C170" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D170" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E170" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F170" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G170" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H170" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J170" s="9" t="s">
         <v>540</v>
-      </c>
-      <c r="D170" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E170" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F170" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G170" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H170" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I170" s="10" t="n">
-        <v>19</v>
-      </c>
-      <c r="J170" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="K170" s="9" t="s">
         <v>541</v>
@@ -8665,45 +8647,45 @@
         <v>542</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>279</v>
+        <v>120</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E171" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F171" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G171" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H171" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="I171" s="10" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J171" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K171" s="9" t="s">
         <v>543</v>
-      </c>
-      <c r="K171" s="9" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="172" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B172" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D172" s="10" t="s">
         <v>16</v>
@@ -8712,69 +8694,69 @@
         <v>17</v>
       </c>
       <c r="F172" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G172" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H172" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="I172" s="10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J172" s="9" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="K172" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="173" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="B173" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C173" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D173" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E173" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F173" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H173" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I173" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J173" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K173" s="9" t="s">
         <v>547</v>
-      </c>
-      <c r="B173" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C173" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D173" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E173" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F173" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G173" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H173" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I173" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J173" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="K173" s="9" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="174" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C174" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="B174" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C174" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="D174" s="10" t="s">
         <v>17</v>
       </c>
@@ -8782,7 +8764,7 @@
         <v>17</v>
       </c>
       <c r="F174" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G174" s="10" t="s">
         <v>17</v>
@@ -8791,30 +8773,30 @@
         <v>16</v>
       </c>
       <c r="I174" s="10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J174" s="9" t="s">
-        <v>140</v>
+        <v>550</v>
       </c>
       <c r="K174" s="9" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="175" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="9" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B175" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>552</v>
+        <v>174</v>
       </c>
       <c r="D175" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E175" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F175" s="10" t="s">
         <v>17</v>
@@ -8823,10 +8805,10 @@
         <v>17</v>
       </c>
       <c r="H175" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I175" s="10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J175" s="9" t="s">
         <v>553</v>
@@ -8840,45 +8822,45 @@
         <v>555</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>174</v>
+        <v>22</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E176" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F176" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G176" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H176" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I176" s="10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J176" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="K176" s="9" t="s">
         <v>556</v>
-      </c>
-      <c r="K176" s="9" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="177" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B177" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="D177" s="10" t="s">
         <v>15</v>
@@ -8896,10 +8878,10 @@
         <v>16</v>
       </c>
       <c r="I177" s="10" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J177" s="9" t="s">
-        <v>515</v>
+        <v>558</v>
       </c>
       <c r="K177" s="9" t="s">
         <v>559</v>
@@ -8910,19 +8892,19 @@
         <v>560</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E178" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F178" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G178" s="10" t="s">
         <v>17</v>
@@ -8931,24 +8913,21 @@
         <v>16</v>
       </c>
       <c r="I178" s="10" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J178" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="K178" s="9" t="s">
-        <v>562</v>
+        <v>457</v>
       </c>
     </row>
     <row r="179" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="9" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="D179" s="10" t="s">
         <v>16</v>
@@ -8957,51 +8936,54 @@
         <v>17</v>
       </c>
       <c r="F179" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="G179" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H179" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I179" s="10" t="n">
         <v>1</v>
       </c>
       <c r="J179" s="9" t="s">
-        <v>457</v>
+        <v>311</v>
+      </c>
+      <c r="K179" s="9" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="180" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C180" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D180" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E180" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G180" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H180" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I180" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="J180" s="9" t="s">
         <v>564</v>
-      </c>
-      <c r="B180" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C180" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D180" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E180" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F180" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G180" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H180" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I180" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J180" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="K180" s="9" t="s">
         <v>565</v>
@@ -9012,16 +8994,16 @@
         <v>566</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E181" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F181" s="10" t="s">
         <v>17</v>
@@ -9033,7 +9015,7 @@
         <v>16</v>
       </c>
       <c r="I181" s="10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J181" s="9" t="s">
         <v>567</v>
@@ -9050,86 +9032,86 @@
         <v>13</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>105</v>
+        <v>174</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E182" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F182" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G182" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H182" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I182" s="10" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J182" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K182" s="9" t="s">
         <v>570</v>
-      </c>
-      <c r="K182" s="9" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="183" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B183" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C183" s="10" t="s">
         <v>572</v>
       </c>
-      <c r="B183" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C183" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="D183" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E183" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F183" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G183" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H183" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I183" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J183" s="9" t="s">
-        <v>50</v>
+        <v>573</v>
       </c>
       <c r="K183" s="9" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="184" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="9" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B184" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>575</v>
+        <v>74</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E184" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F184" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G184" s="10" t="s">
         <v>17</v>
@@ -9138,45 +9120,45 @@
         <v>16</v>
       </c>
       <c r="I184" s="10" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J184" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K184" s="9" t="s">
         <v>576</v>
-      </c>
-      <c r="K184" s="9" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="185" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C185" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E185" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F185" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G185" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H185" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I185" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="J185" s="9" t="s">
         <v>578</v>
-      </c>
-      <c r="B185" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C185" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D185" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E185" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F185" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G185" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H185" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I185" s="10" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J185" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="K185" s="9" t="s">
         <v>579</v>
@@ -9190,16 +9172,16 @@
         <v>13</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>105</v>
+        <v>475</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E186" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F186" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G186" s="10" t="s">
         <v>17</v>
@@ -9208,24 +9190,24 @@
         <v>17</v>
       </c>
       <c r="I186" s="10" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J186" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K186" s="9" t="s">
         <v>581</v>
-      </c>
-      <c r="K186" s="9" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="187" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B187" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>475</v>
+        <v>583</v>
       </c>
       <c r="D187" s="10" t="s">
         <v>16</v>
@@ -9234,7 +9216,7 @@
         <v>17</v>
       </c>
       <c r="F187" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G187" s="10" t="s">
         <v>17</v>
@@ -9243,42 +9225,42 @@
         <v>17</v>
       </c>
       <c r="I187" s="10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J187" s="9" t="s">
-        <v>168</v>
+        <v>584</v>
       </c>
       <c r="K187" s="9" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="188" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="9" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>586</v>
+        <v>60</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E188" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F188" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="G188" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H188" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I188" s="10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J188" s="9" t="s">
         <v>587</v>
@@ -9292,28 +9274,28 @@
         <v>589</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E189" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F189" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G189" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H189" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I189" s="10" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J189" s="9" t="s">
         <v>590</v>
@@ -9330,62 +9312,62 @@
         <v>13</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F190" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G190" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H190" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I190" s="10" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="J190" s="9" t="s">
         <v>593</v>
       </c>
-      <c r="K190" s="9" t="s">
-        <v>594</v>
-      </c>
     </row>
     <row r="191" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B191" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D191" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E191" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F191" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="G191" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H191" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I191" s="10" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="J191" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="K191" s="9" t="s">
         <v>596</v>
       </c>
     </row>
@@ -9394,28 +9376,28 @@
         <v>597</v>
       </c>
       <c r="B192" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E192" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F192" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G192" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H192" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I192" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J192" s="9" t="s">
         <v>598</v>
@@ -9432,16 +9414,16 @@
         <v>37</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>74</v>
+        <v>415</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E193" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F193" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G193" s="10" t="s">
         <v>17</v>
@@ -9450,7 +9432,7 @@
         <v>16</v>
       </c>
       <c r="I193" s="10" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="J193" s="9" t="s">
         <v>601</v>
@@ -9467,16 +9449,16 @@
         <v>37</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>415</v>
+        <v>74</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E194" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F194" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G194" s="10" t="s">
         <v>17</v>
@@ -9485,45 +9467,45 @@
         <v>16</v>
       </c>
       <c r="I194" s="10" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J194" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K194" s="9" t="s">
         <v>604</v>
-      </c>
-      <c r="K194" s="9" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="195" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E195" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F195" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H195" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I195" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J195" s="9" t="s">
         <v>606</v>
-      </c>
-      <c r="B195" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C195" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D195" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E195" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F195" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G195" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H195" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I195" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J195" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="K195" s="9" t="s">
         <v>607</v>
@@ -9534,10 +9516,10 @@
         <v>608</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>105</v>
+        <v>609</v>
       </c>
       <c r="D196" s="10" t="s">
         <v>17</v>
@@ -9546,21 +9528,18 @@
         <v>17</v>
       </c>
       <c r="F196" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G196" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H196" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I196" s="10" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J196" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="K196" s="9" t="s">
         <v>610</v>
       </c>
     </row>
@@ -9569,13 +9548,13 @@
         <v>611</v>
       </c>
       <c r="B197" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C197" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E197" s="10" t="s">
         <v>17</v>
@@ -9587,33 +9566,36 @@
         <v>17</v>
       </c>
       <c r="H197" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I197" s="10" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J197" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="K197" s="9" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="198" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="9" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B198" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>615</v>
+        <v>105</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E198" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F198" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G198" s="10" t="s">
         <v>17</v>
@@ -9622,7 +9604,7 @@
         <v>17</v>
       </c>
       <c r="I198" s="10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J198" s="9" t="s">
         <v>616</v>
@@ -9639,16 +9621,16 @@
         <v>13</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>105</v>
+        <v>619</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E199" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F199" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G199" s="10" t="s">
         <v>17</v>
@@ -9657,30 +9639,30 @@
         <v>17</v>
       </c>
       <c r="I199" s="10" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="J199" s="9" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="K199" s="9" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="200" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="9" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B200" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D200" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E200" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F200" s="10" t="s">
         <v>17</v>
@@ -9689,13 +9671,13 @@
         <v>17</v>
       </c>
       <c r="H200" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I200" s="10" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="J200" s="9" t="s">
-        <v>623</v>
+        <v>553</v>
       </c>
       <c r="K200" s="9" t="s">
         <v>624</v>
@@ -9706,7 +9688,7 @@
         <v>625</v>
       </c>
       <c r="B201" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C201" s="10" t="s">
         <v>626</v>
@@ -9715,7 +9697,7 @@
         <v>17</v>
       </c>
       <c r="E201" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F201" s="10" t="s">
         <v>17</v>
@@ -9727,30 +9709,30 @@
         <v>16</v>
       </c>
       <c r="I201" s="10" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="J201" s="9" t="s">
-        <v>556</v>
+        <v>627</v>
       </c>
       <c r="K201" s="9" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="202" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="202" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D202" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E202" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F202" s="10" t="s">
         <v>17</v>
@@ -9762,14 +9744,12 @@
         <v>16</v>
       </c>
       <c r="I202" s="10" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J202" s="9" t="s">
-        <v>630</v>
-      </c>
-      <c r="K202" s="9" t="s">
         <v>631</v>
       </c>
+      <c r="K202" s="9"/>
     </row>
     <row r="203" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="9" t="s">
@@ -9779,30 +9759,32 @@
         <v>37</v>
       </c>
       <c r="C203" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D203" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E203" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F203" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G203" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H203" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I203" s="10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J203" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="D203" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E203" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F203" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G203" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H203" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I203" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J203" s="9" t="s">
+      <c r="K203" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="K203" s="9"/>
     </row>
     <row r="204" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
@@ -9812,13 +9794,13 @@
         <v>37</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>74</v>
+        <v>636</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E204" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F204" s="10" t="s">
         <v>17</v>
@@ -9830,16 +9812,14 @@
         <v>16</v>
       </c>
       <c r="I204" s="10" t="n">
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="J204" s="9" t="s">
-        <v>636</v>
-      </c>
-      <c r="K204" s="9" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="205" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K204" s="9"/>
+    </row>
+    <row r="205" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="9" t="s">
         <v>638</v>
       </c>
@@ -9847,61 +9827,63 @@
         <v>37</v>
       </c>
       <c r="C205" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D205" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E205" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F205" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G205" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H205" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I205" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J205" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="K205" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="D205" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E205" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F205" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G205" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H205" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I205" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="J205" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="K205" s="9"/>
     </row>
     <row r="206" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C206" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D206" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E206" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F206" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G206" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H206" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I206" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J206" s="9" t="s">
         <v>641</v>
-      </c>
-      <c r="B206" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C206" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D206" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E206" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F206" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G206" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H206" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I206" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J206" s="9" t="s">
-        <v>365</v>
       </c>
       <c r="K206" s="9" t="s">
         <v>642</v>
@@ -9912,28 +9894,28 @@
         <v>643</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E207" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F207" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G207" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H207" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="I207" s="10" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="J207" s="9" t="s">
         <v>644</v>
@@ -9947,10 +9929,10 @@
         <v>646</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>33</v>
+        <v>377</v>
       </c>
       <c r="D208" s="10" t="s">
         <v>17</v>
@@ -9959,7 +9941,7 @@
         <v>16</v>
       </c>
       <c r="F208" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G208" s="10" t="s">
         <v>17</v>
@@ -9968,44 +9950,44 @@
         <v>16</v>
       </c>
       <c r="I208" s="10" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J208" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="K208" s="9" t="s">
-        <v>648</v>
-      </c>
     </row>
     <row r="209" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C209" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D209" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E209" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F209" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G209" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H209" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I209" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J209" s="9" t="s">
         <v>649</v>
       </c>
-      <c r="B209" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C209" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="D209" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E209" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F209" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G209" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H209" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I209" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="J209" s="9" t="s">
+      <c r="K209" s="9" t="s">
         <v>650</v>
       </c>
     </row>
@@ -10014,10 +9996,10 @@
         <v>651</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="C210" s="10" t="s">
-        <v>16</v>
+        <v>174</v>
       </c>
       <c r="D210" s="10" t="s">
         <v>16</v>
@@ -10029,74 +10011,74 @@
         <v>16</v>
       </c>
       <c r="G210" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H210" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I210" s="10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J210" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K210" s="9" t="s">
         <v>652</v>
-      </c>
-      <c r="K210" s="9" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="211" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C211" s="10" t="s">
         <v>654</v>
       </c>
-      <c r="B211" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C211" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="D211" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E211" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F211" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G211" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H211" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I211" s="10" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J211" s="9" t="s">
-        <v>129</v>
+        <v>655</v>
       </c>
       <c r="K211" s="9" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="212" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="9" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B212" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>657</v>
+        <v>222</v>
       </c>
       <c r="D212" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E212" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F212" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G212" s="10" t="s">
         <v>17</v>
@@ -10105,94 +10087,94 @@
         <v>16</v>
       </c>
       <c r="I212" s="10" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J212" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="K212" s="9" t="s">
         <v>658</v>
-      </c>
-      <c r="K212" s="9" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="213" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="B213" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D213" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E213" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F213" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G213" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H213" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I213" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J213" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K213" s="9" t="s">
         <v>660</v>
-      </c>
-      <c r="B213" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C213" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D213" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E213" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F213" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G213" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H213" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I213" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J213" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="K213" s="9" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="214" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C214" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D214" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E214" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F214" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G214" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H214" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I214" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="J214" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="K214" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="B214" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C214" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D214" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E214" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F214" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G214" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H214" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I214" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J214" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="K214" s="9" t="s">
+    </row>
+    <row r="215" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="9" t="s">
         <v>663</v>
-      </c>
-    </row>
-    <row r="215" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="9" t="s">
-        <v>664</v>
       </c>
       <c r="B215" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C215" s="10" t="s">
-        <v>16</v>
+        <v>233</v>
       </c>
       <c r="D215" s="10" t="s">
         <v>17</v>
@@ -10207,71 +10189,69 @@
         <v>17</v>
       </c>
       <c r="H215" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="I215" s="10" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J215" s="9" t="s">
-        <v>480</v>
+        <v>637</v>
       </c>
       <c r="K215" s="9" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="216" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B216" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C216" s="10" t="s">
-        <v>233</v>
+        <v>74</v>
       </c>
       <c r="D216" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E216" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F216" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G216" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H216" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="I216" s="10" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J216" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="K216" s="9" t="s">
-        <v>667</v>
-      </c>
+        <v>666</v>
+      </c>
+      <c r="K216" s="9"/>
     </row>
     <row r="217" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="B217" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217" s="10" t="s">
         <v>668</v>
       </c>
-      <c r="B217" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C217" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="D217" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E217" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F217" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G217" s="10" t="s">
         <v>17</v>
@@ -10280,28 +10260,30 @@
         <v>16</v>
       </c>
       <c r="I217" s="10" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="J217" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K217" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="K217" s="9"/>
     </row>
     <row r="218" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="9" t="s">
         <v>670</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>671</v>
+        <v>377</v>
       </c>
       <c r="D218" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E218" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F218" s="10" t="s">
         <v>17</v>
@@ -10313,33 +10295,31 @@
         <v>16</v>
       </c>
       <c r="I218" s="10" t="n">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="J218" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="K218" s="9" t="s">
-        <v>672</v>
-      </c>
+        <v>647</v>
+      </c>
+      <c r="K218" s="9"/>
     </row>
     <row r="219" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C219" s="10" t="s">
-        <v>377</v>
+        <v>105</v>
       </c>
       <c r="D219" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E219" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F219" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="G219" s="10" t="s">
         <v>17</v>
@@ -10348,16 +10328,18 @@
         <v>16</v>
       </c>
       <c r="I219" s="10" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J219" s="9" t="s">
-        <v>650</v>
-      </c>
-      <c r="K219" s="9"/>
+        <v>168</v>
+      </c>
+      <c r="K219" s="9" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="220" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="9" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B220" s="10" t="s">
         <v>13</v>
@@ -10366,40 +10348,38 @@
         <v>105</v>
       </c>
       <c r="D220" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E220" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F220" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="G220" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H220" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I220" s="10" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J220" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="K220" s="9" t="s">
-        <v>675</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="K220" s="9"/>
     </row>
     <row r="221" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C221" s="10" t="s">
         <v>676</v>
       </c>
-      <c r="B221" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C221" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="D221" s="10" t="s">
         <v>17</v>
       </c>
@@ -10407,13 +10387,13 @@
         <v>17</v>
       </c>
       <c r="F221" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G221" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H221" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I221" s="10" t="n">
         <v>14</v>
@@ -10421,17 +10401,19 @@
       <c r="J221" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="K221" s="9"/>
+      <c r="K221" s="9" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="222" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="9" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>679</v>
+        <v>120</v>
       </c>
       <c r="D222" s="10" t="s">
         <v>17</v>
@@ -10440,16 +10422,16 @@
         <v>17</v>
       </c>
       <c r="F222" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G222" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H222" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I222" s="10" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J222" s="9" t="s">
         <v>680</v>
@@ -10463,10 +10445,10 @@
         <v>682</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D223" s="10" t="s">
         <v>17</v>
@@ -10475,16 +10457,16 @@
         <v>17</v>
       </c>
       <c r="F223" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G223" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H223" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I223" s="10" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J223" s="9" t="s">
         <v>683</v>
@@ -10498,51 +10480,51 @@
         <v>685</v>
       </c>
       <c r="B224" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>128</v>
+        <v>686</v>
       </c>
       <c r="D224" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E224" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F224" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G224" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H224" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I224" s="10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J224" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K224" s="9" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="225" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="9" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B225" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D225" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E225" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F225" s="10" t="s">
         <v>17</v>
@@ -10551,33 +10533,33 @@
         <v>17</v>
       </c>
       <c r="H225" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I225" s="10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J225" s="9" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="K225" s="9" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="226" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="9" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B226" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>693</v>
+        <v>105</v>
       </c>
       <c r="D226" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E226" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F226" s="10" t="s">
         <v>17</v>
@@ -10586,31 +10568,31 @@
         <v>17</v>
       </c>
       <c r="H226" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I226" s="10" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J226" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K226" s="9" t="s">
         <v>694</v>
-      </c>
-      <c r="K226" s="9" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="227" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="B227" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C227" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D227" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="B227" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C227" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D227" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="E227" s="10" t="s">
         <v>17</v>
       </c>
@@ -10621,70 +10603,70 @@
         <v>17</v>
       </c>
       <c r="H227" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I227" s="10" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="J227" s="9" t="s">
-        <v>168</v>
+        <v>697</v>
       </c>
       <c r="K227" s="9" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="228" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="9" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B228" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D228" s="10" t="s">
-        <v>699</v>
-      </c>
-      <c r="E228" s="10" t="s">
-        <v>17</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D228" s="10"/>
+      <c r="E228" s="10"/>
       <c r="F228" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G228" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="H228" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I228" s="10" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J228" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="K228" s="9" t="s">
         <v>700</v>
-      </c>
-      <c r="K228" s="9" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="229" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B229" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D229" s="10"/>
-      <c r="E229" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="D229" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E229" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="F229" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G229" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="H229" s="10" t="s">
         <v>17</v>
@@ -10696,39 +10678,39 @@
         <v>161</v>
       </c>
       <c r="K229" s="9" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="230" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="B230" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C230" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D230" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E230" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F230" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G230" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H230" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I230" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J230" s="9" t="s">
         <v>704</v>
-      </c>
-      <c r="B230" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C230" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D230" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E230" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F230" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G230" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H230" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I230" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J230" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="K230" s="9" t="s">
         <v>705</v>
@@ -10742,16 +10724,16 @@
         <v>37</v>
       </c>
       <c r="C231" s="10" t="s">
-        <v>128</v>
+        <v>423</v>
       </c>
       <c r="D231" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E231" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F231" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G231" s="10" t="s">
         <v>17</v>
@@ -10760,27 +10742,27 @@
         <v>16</v>
       </c>
       <c r="I231" s="10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J231" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K231" s="9" t="s">
         <v>707</v>
-      </c>
-      <c r="K231" s="9" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="232" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="9" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B232" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C232" s="10" t="s">
-        <v>423</v>
+        <v>128</v>
       </c>
       <c r="D232" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E232" s="10" t="s">
         <v>17</v>
@@ -10795,18 +10777,18 @@
         <v>16</v>
       </c>
       <c r="I232" s="10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J232" s="9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K232" s="9" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="233" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="9" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B233" s="10" t="s">
         <v>37</v>
@@ -10815,13 +10797,13 @@
         <v>128</v>
       </c>
       <c r="D233" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E233" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F233" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G233" s="10" t="s">
         <v>17</v>
@@ -10830,16 +10812,16 @@
         <v>16</v>
       </c>
       <c r="I233" s="10" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J233" s="9" t="s">
-        <v>57</v>
+        <v>711</v>
       </c>
       <c r="K233" s="9" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="234" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="9" t="s">
         <v>713</v>
       </c>
@@ -10847,13 +10829,13 @@
         <v>37</v>
       </c>
       <c r="C234" s="10" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="D234" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E234" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F234" s="10" t="s">
         <v>16</v>
@@ -10865,7 +10847,7 @@
         <v>16</v>
       </c>
       <c r="I234" s="10" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J234" s="9" t="s">
         <v>714</v>
@@ -10885,13 +10867,13 @@
         <v>74</v>
       </c>
       <c r="D235" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E235" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F235" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G235" s="10" t="s">
         <v>17</v>
@@ -10900,7 +10882,7 @@
         <v>16</v>
       </c>
       <c r="I235" s="10" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="J235" s="9" t="s">
         <v>717</v>
@@ -10920,13 +10902,13 @@
         <v>74</v>
       </c>
       <c r="D236" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E236" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F236" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G236" s="10" t="s">
         <v>17</v>
@@ -10935,7 +10917,7 @@
         <v>16</v>
       </c>
       <c r="I236" s="10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J236" s="9" t="s">
         <v>720</v>
@@ -10949,13 +10931,13 @@
         <v>722</v>
       </c>
       <c r="B237" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C237" s="10" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="D237" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E237" s="10" t="s">
         <v>17</v>
@@ -10967,10 +10949,10 @@
         <v>17</v>
       </c>
       <c r="H237" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="I237" s="10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J237" s="9" t="s">
         <v>723</v>
@@ -10984,13 +10966,13 @@
         <v>725</v>
       </c>
       <c r="B238" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C238" s="10" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="D238" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E238" s="10" t="s">
         <v>17</v>
@@ -11002,83 +10984,83 @@
         <v>17</v>
       </c>
       <c r="H238" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="I238" s="10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J238" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="K238" s="9" t="s">
         <v>726</v>
-      </c>
-      <c r="K238" s="9" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="239" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="B239" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C239" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D239" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E239" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F239" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G239" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H239" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I239" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J239" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="K239" s="9" t="s">
         <v>728</v>
       </c>
-      <c r="B239" s="10" t="s">
+    </row>
+    <row r="240" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="B240" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C239" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D239" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E239" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F239" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G239" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H239" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I239" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J239" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="K239" s="9" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="240" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="9" t="s">
+      <c r="C240" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D240" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E240" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F240" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G240" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H240" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I240" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J240" s="9" t="s">
         <v>730</v>
-      </c>
-      <c r="B240" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C240" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D240" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E240" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F240" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G240" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H240" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I240" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="J240" s="9" t="s">
-        <v>424</v>
       </c>
       <c r="K240" s="9" t="s">
         <v>731</v>
@@ -11092,7 +11074,7 @@
         <v>37</v>
       </c>
       <c r="C241" s="10" t="s">
-        <v>233</v>
+        <v>150</v>
       </c>
       <c r="D241" s="10" t="s">
         <v>17</v>
@@ -11110,7 +11092,7 @@
         <v>16</v>
       </c>
       <c r="I241" s="10" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="J241" s="9" t="s">
         <v>733</v>
@@ -11133,7 +11115,7 @@
         <v>17</v>
       </c>
       <c r="E242" s="10" t="s">
-        <v>17</v>
+        <v>736</v>
       </c>
       <c r="F242" s="10" t="s">
         <v>16</v>
@@ -11145,16 +11127,16 @@
         <v>16</v>
       </c>
       <c r="I242" s="10" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J242" s="9" t="s">
-        <v>736</v>
+        <v>129</v>
       </c>
       <c r="K242" s="9" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="243" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" s="12" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="9" t="s">
         <v>738</v>
       </c>
@@ -11162,16 +11144,16 @@
         <v>37</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>150</v>
+        <v>739</v>
       </c>
       <c r="D243" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E243" s="10" t="s">
-        <v>739</v>
+        <v>17</v>
       </c>
       <c r="F243" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G243" s="10" t="s">
         <v>17</v>
@@ -11180,24 +11162,24 @@
         <v>16</v>
       </c>
       <c r="I243" s="10" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J243" s="9" t="s">
-        <v>129</v>
+        <v>740</v>
       </c>
       <c r="K243" s="9" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="244" s="12" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="9" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B244" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C244" s="10" t="s">
-        <v>742</v>
+        <v>13</v>
+      </c>
+      <c r="C244" s="13" t="s">
+        <v>743</v>
       </c>
       <c r="D244" s="10" t="s">
         <v>16</v>
@@ -11206,33 +11188,33 @@
         <v>17</v>
       </c>
       <c r="F244" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G244" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H244" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I244" s="10" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J244" s="9" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="K244" s="9" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="245" s="12" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="245" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="9" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B245" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C245" s="13" t="s">
-        <v>746</v>
+      <c r="C245" s="10" t="s">
+        <v>747</v>
       </c>
       <c r="D245" s="10" t="s">
         <v>16</v>
@@ -11250,27 +11232,27 @@
         <v>17</v>
       </c>
       <c r="I245" s="10" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J245" s="9" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="K245" s="9" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="246" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="9" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B246" s="10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>750</v>
+        <v>22</v>
       </c>
       <c r="D246" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E246" s="10" t="s">
         <v>17</v>
@@ -11282,62 +11264,62 @@
         <v>17</v>
       </c>
       <c r="H246" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I246" s="10" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J246" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="K246" s="9" t="s">
         <v>751</v>
-      </c>
-      <c r="K246" s="9" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="247" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="9" t="s">
+        <v>752</v>
+      </c>
+      <c r="B247" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C247" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D247" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E247" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F247" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G247" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H247" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I247" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J247" s="9" t="s">
         <v>753</v>
-      </c>
-      <c r="B247" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C247" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D247" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E247" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F247" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G247" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H247" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I247" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="J247" s="9" t="s">
-        <v>227</v>
       </c>
       <c r="K247" s="9" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="248" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="9" t="s">
         <v>755</v>
       </c>
       <c r="B248" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D248" s="10" t="s">
         <v>17</v>
@@ -11346,7 +11328,7 @@
         <v>17</v>
       </c>
       <c r="F248" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G248" s="10" t="s">
         <v>17</v>
@@ -11358,100 +11340,100 @@
         <v>4</v>
       </c>
       <c r="J248" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="K248" s="9" t="s">
         <v>756</v>
-      </c>
-      <c r="K248" s="9" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="249" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="9" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B249" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="D249" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E249" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F249" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="G249" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H249" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I249" s="10" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="J249" s="9" t="s">
-        <v>372</v>
+        <v>102</v>
       </c>
       <c r="K249" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="250" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="9" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B250" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>128</v>
+        <v>347</v>
       </c>
       <c r="D250" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E250" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F250" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G250" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H250" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I250" s="10" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J250" s="9" t="s">
         <v>102</v>
       </c>
       <c r="K250" s="9" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="251" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="9" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B251" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>347</v>
+        <v>74</v>
       </c>
       <c r="D251" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E251" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F251" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G251" s="10" t="s">
         <v>17</v>
@@ -11460,10 +11442,10 @@
         <v>16</v>
       </c>
       <c r="I251" s="10" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="J251" s="9" t="s">
-        <v>102</v>
+        <v>762</v>
       </c>
       <c r="K251" s="9" t="s">
         <v>763</v>
@@ -11474,28 +11456,28 @@
         <v>764</v>
       </c>
       <c r="B252" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C252" s="10" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="D252" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E252" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F252" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G252" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H252" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I252" s="10" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J252" s="9" t="s">
         <v>765</v>
@@ -11512,7 +11494,7 @@
         <v>13</v>
       </c>
       <c r="C253" s="10" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="D253" s="10" t="s">
         <v>17</v>
@@ -11533,27 +11515,27 @@
         <v>10</v>
       </c>
       <c r="J253" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K253" s="9" t="s">
         <v>768</v>
-      </c>
-      <c r="K253" s="9" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="254" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="9" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B254" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C254" s="10" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D254" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E254" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F254" s="10" t="s">
         <v>17</v>
@@ -11562,48 +11544,48 @@
         <v>17</v>
       </c>
       <c r="H254" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="I254" s="10" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J254" s="9" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="K254" s="9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="255" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="B255" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C255" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D255" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E255" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F255" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G255" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H255" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I255" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="J255" s="9" t="s">
         <v>772</v>
-      </c>
-      <c r="B255" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C255" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D255" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E255" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F255" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G255" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H255" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I255" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="J255" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="K255" s="9" t="s">
         <v>773</v>
@@ -11617,7 +11599,7 @@
         <v>37</v>
       </c>
       <c r="C256" s="10" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
       <c r="D256" s="10" t="s">
         <v>17</v>
@@ -11644,21 +11626,21 @@
         <v>776</v>
       </c>
     </row>
-    <row r="257" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="9" t="s">
         <v>777</v>
       </c>
       <c r="B257" s="10" t="s">
-        <v>37</v>
+        <v>778</v>
       </c>
       <c r="C257" s="10" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D257" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E257" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F257" s="10" t="s">
         <v>17</v>
@@ -11670,24 +11652,77 @@
         <v>16</v>
       </c>
       <c r="I257" s="10" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J257" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="K257" s="9" t="s">
-        <v>779</v>
-      </c>
+        <v>780</v>
+      </c>
+      <c r="L257" s="9"/>
+      <c r="M257" s="9"/>
+      <c r="N257" s="9"/>
+      <c r="O257" s="9"/>
+      <c r="P257" s="9"/>
+      <c r="Q257" s="9"/>
+      <c r="R257" s="9"/>
+      <c r="S257" s="9"/>
+      <c r="T257" s="9"/>
+      <c r="U257" s="9"/>
+      <c r="V257" s="9"/>
+      <c r="W257" s="9"/>
+      <c r="X257" s="9"/>
+      <c r="Y257" s="9"/>
+      <c r="Z257" s="9"/>
+      <c r="AA257" s="9"/>
+      <c r="AB257" s="9"/>
+      <c r="AC257" s="9"/>
+      <c r="AD257" s="9"/>
+      <c r="AE257" s="9"/>
+      <c r="AF257" s="9"/>
+      <c r="AG257" s="9"/>
+      <c r="AH257" s="9"/>
+      <c r="AI257" s="9"/>
+      <c r="AJ257" s="9"/>
+      <c r="AK257" s="9"/>
+      <c r="AL257" s="9"/>
+      <c r="AM257" s="9"/>
+      <c r="AN257" s="9"/>
+      <c r="AO257" s="9"/>
+      <c r="AP257" s="9"/>
+      <c r="AQ257" s="9"/>
+      <c r="AR257" s="9"/>
+      <c r="AS257" s="9"/>
+      <c r="AT257" s="9"/>
+      <c r="AU257" s="9"/>
+      <c r="AV257" s="9"/>
+      <c r="AW257" s="9"/>
+      <c r="AX257" s="9"/>
+      <c r="AY257" s="9"/>
+      <c r="AZ257" s="9"/>
+      <c r="BA257" s="9"/>
+      <c r="BB257" s="9"/>
+      <c r="BC257" s="9"/>
+      <c r="BD257" s="9"/>
+      <c r="BE257" s="9"/>
+      <c r="BF257" s="9"/>
+      <c r="BG257" s="9"/>
+      <c r="BH257" s="9"/>
+      <c r="BI257" s="9"/>
+      <c r="BJ257" s="9"/>
+      <c r="BK257" s="9"/>
+      <c r="BL257" s="9"/>
     </row>
     <row r="258" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="9" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B258" s="10" t="s">
-        <v>781</v>
+        <v>13</v>
       </c>
       <c r="C258" s="10" t="s">
-        <v>16</v>
+        <v>385</v>
       </c>
       <c r="D258" s="10" t="s">
         <v>17</v>
@@ -11696,22 +11731,22 @@
         <v>17</v>
       </c>
       <c r="F258" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G258" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H258" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I258" s="10" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J258" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="K258" s="9" t="s">
         <v>782</v>
-      </c>
-      <c r="K258" s="9" t="s">
-        <v>783</v>
       </c>
       <c r="L258" s="9"/>
       <c r="M258" s="9"/>
@@ -11769,38 +11804,36 @@
     </row>
     <row r="259" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="9" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B259" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C259" s="10" t="s">
-        <v>385</v>
+        <v>16</v>
       </c>
       <c r="D259" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E259" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F259" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G259" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H259" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I259" s="10" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J259" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="K259" s="9" t="s">
-        <v>785</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="K259" s="9"/>
       <c r="L259" s="9"/>
       <c r="M259" s="9"/>
       <c r="N259" s="9"/>
@@ -11857,13 +11890,13 @@
     </row>
     <row r="260" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="9" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C260" s="10" t="s">
-        <v>16</v>
+        <v>630</v>
       </c>
       <c r="D260" s="10" t="s">
         <v>17</v>
@@ -11881,12 +11914,14 @@
         <v>16</v>
       </c>
       <c r="I260" s="10" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="J260" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="K260" s="9"/>
+        <v>276</v>
+      </c>
+      <c r="K260" s="9" t="s">
+        <v>785</v>
+      </c>
       <c r="L260" s="9"/>
       <c r="M260" s="9"/>
       <c r="N260" s="9"/>
@@ -11943,22 +11978,22 @@
     </row>
     <row r="261" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="9" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C261" s="10" t="s">
-        <v>633</v>
+        <v>105</v>
       </c>
       <c r="D261" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E261" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F261" s="10" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="G261" s="10" t="s">
         <v>17</v>
@@ -11970,11 +12005,9 @@
         <v>21</v>
       </c>
       <c r="J261" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="K261" s="9" t="s">
-        <v>788</v>
-      </c>
+        <v>787</v>
+      </c>
+      <c r="K261" s="9"/>
       <c r="L261" s="9"/>
       <c r="M261" s="9"/>
       <c r="N261" s="9"/>
@@ -12031,36 +12064,36 @@
     </row>
     <row r="262" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="B262" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C262" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D262" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E262" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F262" s="10" t="s">
         <v>789</v>
       </c>
-      <c r="B262" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C262" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D262" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E262" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F262" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="G262" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H262" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="H262" s="10"/>
       <c r="I262" s="10" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="J262" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="K262" s="9" t="s">
         <v>790</v>
       </c>
-      <c r="K262" s="9"/>
       <c r="L262" s="9"/>
       <c r="M262" s="9"/>
       <c r="N262" s="9"/>
@@ -12120,29 +12153,31 @@
         <v>791</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C263" s="10" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D263" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E263" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F263" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G263" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H263" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I263" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J263" s="9" t="s">
         <v>792</v>
-      </c>
-      <c r="G263" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H263" s="10"/>
-      <c r="I263" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J263" s="9" t="s">
-        <v>686</v>
       </c>
       <c r="K263" s="9" t="s">
         <v>793</v>
@@ -12209,13 +12244,13 @@
         <v>37</v>
       </c>
       <c r="C264" s="10" t="s">
-        <v>150</v>
+        <v>391</v>
       </c>
       <c r="D264" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E264" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F264" s="10" t="s">
         <v>17</v>
@@ -12227,13 +12262,13 @@
         <v>16</v>
       </c>
       <c r="I264" s="10" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J264" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K264" s="9" t="s">
         <v>795</v>
-      </c>
-      <c r="K264" s="9" t="s">
-        <v>796</v>
       </c>
       <c r="L264" s="9"/>
       <c r="M264" s="9"/>
@@ -12291,22 +12326,22 @@
     </row>
     <row r="265" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="9" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B265" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C265" s="10" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D265" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F265" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G265" s="10" t="s">
         <v>17</v>
@@ -12315,13 +12350,13 @@
         <v>17</v>
       </c>
       <c r="I265" s="10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J265" s="9" t="s">
-        <v>798</v>
+        <v>42</v>
       </c>
       <c r="K265" s="9" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="L265" s="9"/>
       <c r="M265" s="9"/>
@@ -12379,37 +12414,37 @@
     </row>
     <row r="266" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="9" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C266" s="10" t="s">
-        <v>391</v>
+        <v>105</v>
       </c>
       <c r="D266" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E266" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F266" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G266" s="10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="H266" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I266" s="10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J266" s="9" t="s">
         <v>82</v>
       </c>
       <c r="K266" s="9" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="L266" s="9"/>
       <c r="M266" s="9"/>
@@ -12467,38 +12502,36 @@
     </row>
     <row r="267" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="9" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C267" s="10" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="D267" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E267" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F267" s="10" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G267" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H267" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I267" s="10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J267" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K267" s="9" t="s">
-        <v>803</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="K267" s="9"/>
       <c r="L267" s="9"/>
       <c r="M267" s="9"/>
       <c r="N267" s="9"/>
@@ -12555,38 +12588,36 @@
     </row>
     <row r="268" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="9" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C268" s="10" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D268" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E268" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F268" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G268" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="H268" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I268" s="10" t="n">
         <v>3</v>
       </c>
       <c r="J268" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="K268" s="9" t="s">
-        <v>805</v>
-      </c>
+        <v>802</v>
+      </c>
+      <c r="K268" s="9"/>
       <c r="L268" s="9"/>
       <c r="M268" s="9"/>
       <c r="N268" s="9"/>
@@ -12643,13 +12674,13 @@
     </row>
     <row r="269" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="9" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C269" s="10" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="D269" s="10" t="s">
         <v>16</v>
@@ -12658,19 +12689,19 @@
         <v>17</v>
       </c>
       <c r="F269" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G269" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H269" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I269" s="10" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="J269" s="9" t="s">
-        <v>276</v>
+        <v>804</v>
       </c>
       <c r="K269" s="9"/>
       <c r="L269" s="9"/>
@@ -12729,22 +12760,22 @@
     </row>
     <row r="270" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="9" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B270" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C270" s="10" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="D270" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E270" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F270" s="10" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G270" s="10" t="s">
         <v>17</v>
@@ -12753,12 +12784,14 @@
         <v>16</v>
       </c>
       <c r="I270" s="10" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J270" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="K270" s="9"/>
+        <v>102</v>
+      </c>
+      <c r="K270" s="9" t="s">
+        <v>806</v>
+      </c>
       <c r="L270" s="9"/>
       <c r="M270" s="9"/>
       <c r="N270" s="9"/>
@@ -12815,36 +12848,38 @@
     </row>
     <row r="271" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="B271" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C271" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D271" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E271" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F271" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G271" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H271" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I271" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="J271" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="K271" s="9" t="s">
         <v>809</v>
       </c>
-      <c r="B271" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C271" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D271" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E271" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F271" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G271" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H271" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I271" s="10" t="n">
-        <v>31</v>
-      </c>
-      <c r="J271" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="K271" s="9"/>
       <c r="L271" s="9"/>
       <c r="M271" s="9"/>
       <c r="N271" s="9"/>
@@ -12901,7 +12936,7 @@
     </row>
     <row r="272" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B272" s="10" t="s">
         <v>37</v>
@@ -12910,13 +12945,13 @@
         <v>16</v>
       </c>
       <c r="D272" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E272" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F272" s="10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="G272" s="10" t="s">
         <v>17</v>
@@ -12925,13 +12960,13 @@
         <v>16</v>
       </c>
       <c r="I272" s="10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J272" s="9" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="K272" s="9" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="L272" s="9"/>
       <c r="M272" s="9"/>
@@ -12989,37 +13024,37 @@
     </row>
     <row r="273" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="B273" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C273" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D273" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E273" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F273" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G273" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H273" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I273" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J273" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="K273" s="9" t="s">
         <v>813</v>
-      </c>
-      <c r="B273" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C273" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D273" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E273" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F273" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G273" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H273" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I273" s="10" t="n">
-        <v>16</v>
-      </c>
-      <c r="J273" s="9" t="s">
-        <v>814</v>
-      </c>
-      <c r="K273" s="9" t="s">
-        <v>815</v>
       </c>
       <c r="L273" s="9"/>
       <c r="M273" s="9"/>
@@ -13077,13 +13112,13 @@
     </row>
     <row r="274" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="9" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C274" s="10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D274" s="10" t="s">
         <v>17</v>
@@ -13092,7 +13127,7 @@
         <v>16</v>
       </c>
       <c r="F274" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G274" s="10" t="s">
         <v>17</v>
@@ -13101,13 +13136,13 @@
         <v>16</v>
       </c>
       <c r="I274" s="10" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J274" s="9" t="s">
-        <v>42</v>
+        <v>311</v>
       </c>
       <c r="K274" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="L274" s="9"/>
       <c r="M274" s="9"/>
@@ -13165,22 +13200,22 @@
     </row>
     <row r="275" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="9" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B275" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C275" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D275" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E275" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F275" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G275" s="10" t="s">
         <v>17</v>
@@ -13189,13 +13224,13 @@
         <v>17</v>
       </c>
       <c r="I275" s="10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J275" s="9" t="s">
-        <v>814</v>
+        <v>311</v>
       </c>
       <c r="K275" s="9" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="L275" s="9"/>
       <c r="M275" s="9"/>
@@ -13253,19 +13288,19 @@
     </row>
     <row r="276" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="9" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B276" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C276" s="10" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="D276" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E276" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F276" s="10" t="s">
         <v>16</v>
@@ -13277,13 +13312,13 @@
         <v>16</v>
       </c>
       <c r="I276" s="10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J276" s="9" t="s">
-        <v>311</v>
+        <v>683</v>
       </c>
       <c r="K276" s="9" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="L276" s="9"/>
       <c r="M276" s="9"/>
@@ -13339,183 +13374,6 @@
       <c r="BK276" s="9"/>
       <c r="BL276" s="9"/>
     </row>
-    <row r="277" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="9" t="s">
-        <v>822</v>
-      </c>
-      <c r="B277" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C277" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D277" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E277" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F277" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G277" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H277" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I277" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J277" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="K277" s="9" t="s">
-        <v>823</v>
-      </c>
-      <c r="L277" s="9"/>
-      <c r="M277" s="9"/>
-      <c r="N277" s="9"/>
-      <c r="O277" s="9"/>
-      <c r="P277" s="9"/>
-      <c r="Q277" s="9"/>
-      <c r="R277" s="9"/>
-      <c r="S277" s="9"/>
-      <c r="T277" s="9"/>
-      <c r="U277" s="9"/>
-      <c r="V277" s="9"/>
-      <c r="W277" s="9"/>
-      <c r="X277" s="9"/>
-      <c r="Y277" s="9"/>
-      <c r="Z277" s="9"/>
-      <c r="AA277" s="9"/>
-      <c r="AB277" s="9"/>
-      <c r="AC277" s="9"/>
-      <c r="AD277" s="9"/>
-      <c r="AE277" s="9"/>
-      <c r="AF277" s="9"/>
-      <c r="AG277" s="9"/>
-      <c r="AH277" s="9"/>
-      <c r="AI277" s="9"/>
-      <c r="AJ277" s="9"/>
-      <c r="AK277" s="9"/>
-      <c r="AL277" s="9"/>
-      <c r="AM277" s="9"/>
-      <c r="AN277" s="9"/>
-      <c r="AO277" s="9"/>
-      <c r="AP277" s="9"/>
-      <c r="AQ277" s="9"/>
-      <c r="AR277" s="9"/>
-      <c r="AS277" s="9"/>
-      <c r="AT277" s="9"/>
-      <c r="AU277" s="9"/>
-      <c r="AV277" s="9"/>
-      <c r="AW277" s="9"/>
-      <c r="AX277" s="9"/>
-      <c r="AY277" s="9"/>
-      <c r="AZ277" s="9"/>
-      <c r="BA277" s="9"/>
-      <c r="BB277" s="9"/>
-      <c r="BC277" s="9"/>
-      <c r="BD277" s="9"/>
-      <c r="BE277" s="9"/>
-      <c r="BF277" s="9"/>
-      <c r="BG277" s="9"/>
-      <c r="BH277" s="9"/>
-      <c r="BI277" s="9"/>
-      <c r="BJ277" s="9"/>
-      <c r="BK277" s="9"/>
-      <c r="BL277" s="9"/>
-    </row>
-    <row r="278" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="9" t="s">
-        <v>824</v>
-      </c>
-      <c r="B278" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C278" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D278" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E278" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F278" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G278" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H278" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I278" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J278" s="9" t="s">
-        <v>686</v>
-      </c>
-      <c r="K278" s="9" t="s">
-        <v>825</v>
-      </c>
-      <c r="L278" s="9"/>
-      <c r="M278" s="9"/>
-      <c r="N278" s="9"/>
-      <c r="O278" s="9"/>
-      <c r="P278" s="9"/>
-      <c r="Q278" s="9"/>
-      <c r="R278" s="9"/>
-      <c r="S278" s="9"/>
-      <c r="T278" s="9"/>
-      <c r="U278" s="9"/>
-      <c r="V278" s="9"/>
-      <c r="W278" s="9"/>
-      <c r="X278" s="9"/>
-      <c r="Y278" s="9"/>
-      <c r="Z278" s="9"/>
-      <c r="AA278" s="9"/>
-      <c r="AB278" s="9"/>
-      <c r="AC278" s="9"/>
-      <c r="AD278" s="9"/>
-      <c r="AE278" s="9"/>
-      <c r="AF278" s="9"/>
-      <c r="AG278" s="9"/>
-      <c r="AH278" s="9"/>
-      <c r="AI278" s="9"/>
-      <c r="AJ278" s="9"/>
-      <c r="AK278" s="9"/>
-      <c r="AL278" s="9"/>
-      <c r="AM278" s="9"/>
-      <c r="AN278" s="9"/>
-      <c r="AO278" s="9"/>
-      <c r="AP278" s="9"/>
-      <c r="AQ278" s="9"/>
-      <c r="AR278" s="9"/>
-      <c r="AS278" s="9"/>
-      <c r="AT278" s="9"/>
-      <c r="AU278" s="9"/>
-      <c r="AV278" s="9"/>
-      <c r="AW278" s="9"/>
-      <c r="AX278" s="9"/>
-      <c r="AY278" s="9"/>
-      <c r="AZ278" s="9"/>
-      <c r="BA278" s="9"/>
-      <c r="BB278" s="9"/>
-      <c r="BC278" s="9"/>
-      <c r="BD278" s="9"/>
-      <c r="BE278" s="9"/>
-      <c r="BF278" s="9"/>
-      <c r="BG278" s="9"/>
-      <c r="BH278" s="9"/>
-      <c r="BI278" s="9"/>
-      <c r="BJ278" s="9"/>
-      <c r="BK278" s="9"/>
-      <c r="BL278" s="9"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="J:J"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13537,7 +13395,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="1:276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13547,27 +13405,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>